<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@cfca4da2b2d8e9e77384048080f8f4f959c73574 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-tnm-distant-metastases-category.xlsx
+++ b/StructureDefinition-tnm-distant-metastases-category.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$62</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2411" uniqueCount="506">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-08T13:30:59+00:00</t>
+    <t>2024-04-08T16:49:27+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -653,6 +653,14 @@
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
   </si>
   <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://loinc.org"/&gt;
+    &lt;code value="33732-9"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
+  </si>
+  <si>
     <t>http://idg-rlp.de/fhir/tumorkonferenzen/ValueSet/tnm-distant-metastases-staging-type-vs</t>
   </si>
   <si>
@@ -731,7 +739,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Encounter)
+    <t xml:space="preserve">Reference(http://idg-rlp.de/fhir/tumorkonferenzen/StructureDefinition/verlauf)
 </t>
   </si>
   <si>
@@ -766,8 +774,8 @@
 </t>
   </si>
   <si>
-    <t>dateTime
-PeriodTiminginstant</t>
+    <t xml:space="preserve">dateTime
+</t>
   </si>
   <si>
     <t>Clinically relevant time/time-period for observation</t>
@@ -862,7 +870,7 @@
     <t>An observation exists to have a value, though it might not if it is in error, or if it represents a group of observations.</t>
   </si>
   <si>
-    <t>http://idg-rlp.de/fhir/tumorkonferenzen/ValueSet/tnm-distant-metastases-category-vs</t>
+    <t>http://idg-rlp.de/fhir/tumorkonferenzen/ValueSet/HistoGradeVS</t>
   </si>
   <si>
     <t xml:space="preserve">obs-7
@@ -881,6 +889,217 @@
     <t>363714003 |Interprets|</t>
   </si>
   <si>
+    <t>Observation.value[x].id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Observation.value[x].extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>Observation.value[x].coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding
+</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>C*E.1-8, C*E.10-22</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>Observation.value[x].coding.id</t>
+  </si>
+  <si>
+    <t>Observation.value[x].coding.extension</t>
+  </si>
+  <si>
+    <t>Observation.value[x].coding.system</t>
+  </si>
+  <si>
+    <t>Identity of the terminology system</t>
+  </si>
+  <si>
+    <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
+  </si>
+  <si>
+    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should reference to some definition that establishes the system clearly and unambiguously.</t>
+  </si>
+  <si>
+    <t>Need to be unambiguous about the source of the definition of the symbol.</t>
+  </si>
+  <si>
+    <t>Coding.system</t>
+  </si>
+  <si>
+    <t>C*E.3</t>
+  </si>
+  <si>
+    <t>./codeSystem</t>
+  </si>
+  <si>
+    <t>Observation.value[x].coding.version</t>
+  </si>
+  <si>
+    <t>Version of the system - if relevant</t>
+  </si>
+  <si>
+    <t>The version of the code system which was used when choosing this code. Note that a well-maintained code system does not need the version reported, because the meaning of codes is consistent across versions. However this cannot consistently be assured, and when the meaning is not guaranteed to be consistent, the version SHOULD be exchanged.</t>
+  </si>
+  <si>
+    <t>Where the terminology does not clearly define what string should be used to identify code system versions, the recommendation is to use the date (expressed in FHIR date format) on which that version was officially published as the version date.</t>
+  </si>
+  <si>
+    <t>Coding.version</t>
+  </si>
+  <si>
+    <t>C*E.7</t>
+  </si>
+  <si>
+    <t>./codeSystemVersion</t>
+  </si>
+  <si>
+    <t>Observation.value[x].coding.code</t>
+  </si>
+  <si>
+    <t>Symbol in syntax defined by the system</t>
+  </si>
+  <si>
+    <t>A symbol in syntax defined by the system. The symbol may be a predefined code or an expression in a syntax defined by the coding system (e.g. post-coordination).</t>
+  </si>
+  <si>
+    <t>Need to refer to a particular code in the system.</t>
+  </si>
+  <si>
+    <t>Coding.code</t>
+  </si>
+  <si>
+    <t>C*E.1</t>
+  </si>
+  <si>
+    <t>./code</t>
+  </si>
+  <si>
+    <t>Observation.value[x].coding.display</t>
+  </si>
+  <si>
+    <t>Representation defined by the system</t>
+  </si>
+  <si>
+    <t>A representation of the meaning of the code in the system, following the rules of the system.</t>
+  </si>
+  <si>
+    <t>Need to be able to carry a human-readable meaning of the code for readers that do not know  the system.</t>
+  </si>
+  <si>
+    <t>Coding.display</t>
+  </si>
+  <si>
+    <t>C*E.2 - but note this is not well followed</t>
+  </si>
+  <si>
+    <t>CV.displayName</t>
+  </si>
+  <si>
+    <t>Observation.value[x].coding.userSelected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean
+</t>
+  </si>
+  <si>
+    <t>If this coding was chosen directly by the user</t>
+  </si>
+  <si>
+    <t>Indicates that this coding was chosen by a user directly - e.g. off a pick list of available items (codes or displays).</t>
+  </si>
+  <si>
+    <t>Amongst a set of alternatives, a directly chosen code is the most appropriate starting point for new translations. There is some ambiguity about what exactly 'directly chosen' implies, and trading partner agreement may be needed to clarify the use of this element and its consequences more completely.</t>
+  </si>
+  <si>
+    <t>This has been identified as a clinical safety criterium - that this exact system/code pair was chosen explicitly, rather than inferred by the system based on some rules or language processing.</t>
+  </si>
+  <si>
+    <t>Coding.userSelected</t>
+  </si>
+  <si>
+    <t>Sometimes implied by being first</t>
+  </si>
+  <si>
+    <t>CD.codingRationale</t>
+  </si>
+  <si>
+    <t>Observation.value[x].text</t>
+  </si>
+  <si>
+    <t>Plain text representation of the concept</t>
+  </si>
+  <si>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
+    <t>Very often the text is the same as a displayName of one of the codings.</t>
+  </si>
+  <si>
+    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.text</t>
+  </si>
+  <si>
+    <t>C*E.9. But note many systems use C*E.2 for this</t>
+  </si>
+  <si>
+    <t>./originalText[mediaType/code="text/plain"]/data</t>
+  </si>
+  <si>
     <t>Observation.dataAbsentReason</t>
   </si>
   <si>
@@ -1115,29 +1334,7 @@
     <t>Observation.referenceRange.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string
-</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Observation.referenceRange.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
   </si>
   <si>
     <t>Observation.referenceRange.modifierExtension</t>
@@ -1714,7 +1911,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP51"/>
+  <dimension ref="A1:AP62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1751,7 +1948,7 @@
     <col min="26" max="26" width="82.99609375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="41.01953125" customWidth="true" bestFit="true" hidden="true"/>
@@ -3628,7 +3825,7 @@
         <v>80</v>
       </c>
       <c r="S16" t="s" s="2">
-        <v>80</v>
+        <v>204</v>
       </c>
       <c r="T16" t="s" s="2">
         <v>80</v>
@@ -3647,7 +3844,7 @@
       </c>
       <c r="Y16" s="2"/>
       <c r="Z16" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>80</v>
@@ -3680,30 +3877,30 @@
         <v>103</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AP16" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3711,7 +3908,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>91</v>
@@ -3726,19 +3923,19 @@
         <v>92</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>80</v>
@@ -3787,7 +3984,7 @@
         <v>80</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>78</v>
@@ -3802,19 +3999,19 @@
         <v>103</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AP17" t="s" s="2">
         <v>80</v>
@@ -3822,10 +4019,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3848,16 +4045,16 @@
         <v>92</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
@@ -3907,7 +4104,7 @@
         <v>80</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>78</v>
@@ -3928,13 +4125,13 @@
         <v>80</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AP18" t="s" s="2">
         <v>80</v>
@@ -3942,14 +4139,14 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
@@ -3959,7 +4156,7 @@
         <v>91</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>80</v>
@@ -3968,19 +4165,19 @@
         <v>92</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>80</v>
@@ -4029,7 +4226,7 @@
         <v>80</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>78</v>
@@ -4044,19 +4241,19 @@
         <v>103</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AP19" t="s" s="2">
         <v>80</v>
@@ -4064,14 +4261,14 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
@@ -4090,19 +4287,19 @@
         <v>92</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>80</v>
@@ -4151,7 +4348,7 @@
         <v>80</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>78</v>
@@ -4166,19 +4363,19 @@
         <v>103</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AP20" t="s" s="2">
         <v>80</v>
@@ -4186,10 +4383,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4212,16 +4409,16 @@
         <v>92</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -4271,7 +4468,7 @@
         <v>80</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>78</v>
@@ -4292,13 +4489,13 @@
         <v>80</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AP21" t="s" s="2">
         <v>80</v>
@@ -4306,10 +4503,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4332,17 +4529,17 @@
         <v>92</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>80</v>
@@ -4391,7 +4588,7 @@
         <v>80</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -4406,19 +4603,19 @@
         <v>103</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AP22" t="s" s="2">
         <v>80</v>
@@ -4426,10 +4623,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4437,7 +4634,7 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>91</v>
@@ -4455,16 +4652,16 @@
         <v>189</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>80</v>
@@ -4489,11 +4686,11 @@
         <v>80</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>115</v>
+        <v>180</v>
       </c>
       <c r="Y23" s="2"/>
       <c r="Z23" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>80</v>
@@ -4511,7 +4708,7 @@
         <v>80</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>78</v>
@@ -4520,7 +4717,7 @@
         <v>91</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>103</v>
@@ -4529,27 +4726,27 @@
         <v>80</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP23" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4572,20 +4769,16 @@
         <v>80</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>189</v>
+        <v>279</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="O24" t="s" s="2">
         <v>281</v>
       </c>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
         <v>80</v>
       </c>
@@ -4609,31 +4802,31 @@
         <v>80</v>
       </c>
       <c r="X24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE24" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF24" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="Y24" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="Z24" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="AA24" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AB24" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC24" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AD24" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AE24" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AF24" t="s" s="2">
-        <v>277</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>78</v>
@@ -4642,10 +4835,10 @@
         <v>91</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>285</v>
+        <v>80</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>80</v>
@@ -4654,10 +4847,10 @@
         <v>80</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>80</v>
@@ -4668,14 +4861,14 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>288</v>
+        <v>136</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4694,20 +4887,18 @@
         <v>80</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>189</v>
+        <v>137</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>289</v>
+        <v>138</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="O25" t="s" s="2">
-        <v>292</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
         <v>80</v>
       </c>
@@ -4731,31 +4922,31 @@
         <v>80</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>282</v>
+        <v>80</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="Z25" t="s" s="2">
-        <v>294</v>
+        <v>80</v>
       </c>
       <c r="AA25" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AB25" t="s" s="2">
-        <v>80</v>
+        <v>286</v>
       </c>
       <c r="AC25" t="s" s="2">
-        <v>80</v>
+        <v>287</v>
       </c>
       <c r="AD25" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>80</v>
+        <v>288</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>78</v>
@@ -4767,33 +4958,33 @@
         <v>80</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>295</v>
+        <v>80</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>296</v>
+        <v>80</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP25" t="s" s="2">
-        <v>298</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4801,34 +4992,34 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>79</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I26" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>80</v>
@@ -4877,7 +5068,7 @@
         <v>80</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
@@ -4898,10 +5089,10 @@
         <v>80</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>80</v>
@@ -4912,10 +5103,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4938,17 +5129,15 @@
         <v>80</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>189</v>
+        <v>279</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>310</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
         <v>80</v>
@@ -4973,13 +5162,13 @@
         <v>80</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>311</v>
+        <v>80</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>312</v>
+        <v>80</v>
       </c>
       <c r="Z27" t="s" s="2">
-        <v>313</v>
+        <v>80</v>
       </c>
       <c r="AA27" t="s" s="2">
         <v>80</v>
@@ -4997,7 +5186,7 @@
         <v>80</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
@@ -5009,47 +5198,47 @@
         <v>80</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>314</v>
+        <v>80</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>315</v>
+        <v>80</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP27" t="s" s="2">
-        <v>317</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="I28" t="s" s="2">
         <v>80</v>
@@ -5058,20 +5247,18 @@
         <v>80</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>189</v>
+        <v>137</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>319</v>
+        <v>138</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>320</v>
+        <v>285</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="O28" t="s" s="2">
-        <v>322</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
         <v>80</v>
       </c>
@@ -5095,41 +5282,43 @@
         <v>80</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="Y28" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="Y28" t="s" s="2">
+        <v>80</v>
+      </c>
       <c r="Z28" t="s" s="2">
-        <v>323</v>
+        <v>80</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AB28" t="s" s="2">
-        <v>80</v>
+        <v>286</v>
       </c>
       <c r="AC28" t="s" s="2">
-        <v>80</v>
+        <v>287</v>
       </c>
       <c r="AD28" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>80</v>
+        <v>288</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>318</v>
+        <v>289</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>80</v>
@@ -5138,10 +5327,10 @@
         <v>80</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>324</v>
+        <v>80</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>325</v>
+        <v>283</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>80</v>
@@ -5152,10 +5341,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5163,33 +5352,35 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>91</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I29" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>327</v>
+        <v>105</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>328</v>
+        <v>302</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>329</v>
+        <v>303</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="O29" s="2"/>
+        <v>304</v>
+      </c>
+      <c r="O29" t="s" s="2">
+        <v>305</v>
+      </c>
       <c r="P29" t="s" s="2">
         <v>80</v>
       </c>
@@ -5237,7 +5428,7 @@
         <v>80</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -5255,27 +5446,27 @@
         <v>80</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>331</v>
+        <v>80</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>332</v>
+        <v>307</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>333</v>
+        <v>308</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP29" t="s" s="2">
-        <v>334</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5295,19 +5486,19 @@
         <v>80</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>336</v>
+        <v>279</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>339</v>
+        <v>312</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5357,7 +5548,7 @@
         <v>80</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>335</v>
+        <v>313</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
@@ -5375,27 +5566,27 @@
         <v>80</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>340</v>
+        <v>80</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="AO30" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP30" t="s" s="2">
-        <v>343</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>344</v>
+        <v>316</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>344</v>
+        <v>316</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5403,34 +5594,32 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>345</v>
+        <v>111</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>346</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
-        <v>347</v>
+        <v>319</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>80</v>
@@ -5479,19 +5668,19 @@
         <v>80</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="AI31" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>348</v>
+        <v>103</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>80</v>
@@ -5500,10 +5689,10 @@
         <v>80</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>349</v>
+        <v>321</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>350</v>
+        <v>322</v>
       </c>
       <c r="AO31" t="s" s="2">
         <v>80</v>
@@ -5514,10 +5703,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5537,19 +5726,21 @@
         <v>80</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>352</v>
+        <v>279</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>353</v>
+        <v>324</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>354</v>
+        <v>325</v>
       </c>
       <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
+      <c r="O32" t="s" s="2">
+        <v>326</v>
+      </c>
       <c r="P32" t="s" s="2">
         <v>80</v>
       </c>
@@ -5597,7 +5788,7 @@
         <v>80</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>355</v>
+        <v>327</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5609,7 +5800,7 @@
         <v>80</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>80</v>
@@ -5618,10 +5809,10 @@
         <v>80</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>80</v>
+        <v>328</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>80</v>
@@ -5632,21 +5823,21 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>357</v>
+        <v>330</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>357</v>
+        <v>330</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>80</v>
@@ -5655,21 +5846,23 @@
         <v>80</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>137</v>
+        <v>331</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>138</v>
+        <v>332</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="O33" s="2"/>
+        <v>334</v>
+      </c>
+      <c r="O33" t="s" s="2">
+        <v>335</v>
+      </c>
       <c r="P33" t="s" s="2">
         <v>80</v>
       </c>
@@ -5717,19 +5910,19 @@
         <v>80</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>359</v>
+        <v>336</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>80</v>
@@ -5738,10 +5931,10 @@
         <v>80</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>80</v>
+        <v>337</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>356</v>
+        <v>338</v>
       </c>
       <c r="AO33" t="s" s="2">
         <v>80</v>
@@ -5752,45 +5945,45 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>361</v>
+        <v>80</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="J34" t="s" s="2">
         <v>92</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>137</v>
+        <v>279</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>362</v>
+        <v>340</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>140</v>
+        <v>342</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>146</v>
+        <v>343</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>80</v>
@@ -5839,19 +6032,19 @@
         <v>80</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>80</v>
@@ -5860,10 +6053,10 @@
         <v>80</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>80</v>
+        <v>345</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>134</v>
+        <v>346</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>80</v>
@@ -5874,10 +6067,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5900,16 +6093,20 @@
         <v>80</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>366</v>
+        <v>189</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
+        <v>349</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="O35" t="s" s="2">
+        <v>351</v>
+      </c>
       <c r="P35" t="s" s="2">
         <v>80</v>
       </c>
@@ -5933,13 +6130,13 @@
         <v>80</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>80</v>
+        <v>352</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>80</v>
+        <v>353</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>80</v>
+        <v>354</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>80</v>
@@ -5957,7 +6154,7 @@
         <v>80</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>78</v>
@@ -5966,7 +6163,7 @@
         <v>91</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>103</v>
@@ -5978,10 +6175,10 @@
         <v>80</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>370</v>
+        <v>134</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>80</v>
@@ -5992,21 +6189,21 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>80</v>
+        <v>358</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>80</v>
@@ -6018,16 +6215,20 @@
         <v>80</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>366</v>
+        <v>189</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>374</v>
-      </c>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
+        <v>360</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="O36" t="s" s="2">
+        <v>362</v>
+      </c>
       <c r="P36" t="s" s="2">
         <v>80</v>
       </c>
@@ -6051,13 +6252,13 @@
         <v>80</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>80</v>
+        <v>352</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>80</v>
+        <v>363</v>
       </c>
       <c r="Z36" t="s" s="2">
-        <v>80</v>
+        <v>364</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>80</v>
@@ -6075,16 +6276,16 @@
         <v>80</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>369</v>
+        <v>80</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>103</v>
@@ -6093,27 +6294,27 @@
         <v>80</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>80</v>
+        <v>365</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP36" t="s" s="2">
-        <v>80</v>
+        <v>368</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6124,7 +6325,7 @@
         <v>78</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>80</v>
@@ -6136,19 +6337,19 @@
         <v>80</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>189</v>
+        <v>370</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>80</v>
@@ -6173,13 +6374,13 @@
         <v>80</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>381</v>
+        <v>80</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>382</v>
+        <v>80</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>80</v>
@@ -6197,13 +6398,13 @@
         <v>80</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>80</v>
@@ -6215,13 +6416,13 @@
         <v>80</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>383</v>
+        <v>80</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>297</v>
+        <v>376</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>80</v>
@@ -6232,10 +6433,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6246,7 +6447,7 @@
         <v>78</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>80</v>
@@ -6261,17 +6462,15 @@
         <v>189</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>389</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
         <v>80</v>
       </c>
@@ -6295,13 +6494,13 @@
         <v>80</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>311</v>
+        <v>381</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>80</v>
@@ -6319,13 +6518,13 @@
         <v>80</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>80</v>
@@ -6337,27 +6536,27 @@
         <v>80</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>297</v>
+        <v>386</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP38" t="s" s="2">
-        <v>80</v>
+        <v>387</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6365,13 +6564,13 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>91</v>
       </c>
       <c r="H39" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I39" t="s" s="2">
         <v>80</v>
@@ -6380,17 +6579,19 @@
         <v>80</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>393</v>
+        <v>189</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="N39" s="2"/>
+        <v>390</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>391</v>
+      </c>
       <c r="O39" t="s" s="2">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>80</v>
@@ -6415,13 +6616,11 @@
         <v>80</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Y39" t="s" s="2">
-        <v>80</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="Y39" s="2"/>
       <c r="Z39" t="s" s="2">
-        <v>80</v>
+        <v>393</v>
       </c>
       <c r="AA39" t="s" s="2">
         <v>80</v>
@@ -6439,7 +6638,7 @@
         <v>80</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>78</v>
@@ -6460,10 +6659,10 @@
         <v>80</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>80</v>
+        <v>394</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>80</v>
@@ -6474,10 +6673,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6500,15 +6699,17 @@
         <v>80</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>352</v>
+        <v>397</v>
       </c>
       <c r="L40" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="M40" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="M40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
         <v>80</v>
@@ -6557,7 +6758,7 @@
         <v>80</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>78</v>
@@ -6575,27 +6776,27 @@
         <v>80</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>80</v>
+        <v>401</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>370</v>
+        <v>402</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP40" t="s" s="2">
-        <v>80</v>
+        <v>404</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6606,7 +6807,7 @@
         <v>78</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>80</v>
@@ -6615,19 +6816,19 @@
         <v>80</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>337</v>
+        <v>407</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>338</v>
+        <v>408</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -6677,13 +6878,13 @@
         <v>80</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="AI41" t="s" s="2">
         <v>80</v>
@@ -6695,27 +6896,27 @@
         <v>80</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>80</v>
+        <v>410</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP41" t="s" s="2">
-        <v>80</v>
+        <v>413</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6735,21 +6936,23 @@
         <v>80</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="M42" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="L42" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>410</v>
-      </c>
       <c r="N42" t="s" s="2">
-        <v>411</v>
-      </c>
-      <c r="O42" s="2"/>
+        <v>416</v>
+      </c>
+      <c r="O42" t="s" s="2">
+        <v>417</v>
+      </c>
       <c r="P42" t="s" s="2">
         <v>80</v>
       </c>
@@ -6797,7 +7000,7 @@
         <v>80</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
@@ -6809,7 +7012,7 @@
         <v>80</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>103</v>
+        <v>418</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>80</v>
@@ -6818,10 +7021,10 @@
         <v>80</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>412</v>
+        <v>420</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>80</v>
@@ -6832,10 +7035,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6846,7 +7049,7 @@
         <v>78</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>80</v>
@@ -6855,23 +7058,19 @@
         <v>80</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>345</v>
+        <v>279</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>414</v>
+        <v>280</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>416</v>
-      </c>
-      <c r="O43" t="s" s="2">
-        <v>417</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
         <v>80</v>
       </c>
@@ -6919,19 +7118,19 @@
         <v>80</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>413</v>
+        <v>282</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>80</v>
@@ -6940,10 +7139,10 @@
         <v>80</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>418</v>
+        <v>80</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>419</v>
+        <v>283</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>80</v>
@@ -6954,21 +7153,21 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>80</v>
@@ -6980,15 +7179,17 @@
         <v>80</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>352</v>
+        <v>137</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>353</v>
+        <v>138</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="N44" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>140</v>
+      </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
         <v>80</v>
@@ -7037,19 +7238,19 @@
         <v>80</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>355</v>
+        <v>289</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>80</v>
@@ -7061,7 +7262,7 @@
         <v>80</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>356</v>
+        <v>283</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>80</v>
@@ -7072,14 +7273,14 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>136</v>
+        <v>424</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
@@ -7092,24 +7293,26 @@
         <v>80</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K45" t="s" s="2">
         <v>137</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>138</v>
+        <v>425</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>358</v>
+        <v>426</v>
       </c>
       <c r="N45" t="s" s="2">
         <v>140</v>
       </c>
-      <c r="O45" s="2"/>
+      <c r="O45" t="s" s="2">
+        <v>146</v>
+      </c>
       <c r="P45" t="s" s="2">
         <v>80</v>
       </c>
@@ -7157,7 +7360,7 @@
         <v>80</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>359</v>
+        <v>427</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>78</v>
@@ -7181,7 +7384,7 @@
         <v>80</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>356</v>
+        <v>134</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>80</v>
@@ -7192,46 +7395,42 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>361</v>
+        <v>80</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>137</v>
+        <v>429</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>362</v>
+        <v>430</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="O46" t="s" s="2">
-        <v>146</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>80</v>
       </c>
@@ -7279,19 +7478,19 @@
         <v>80</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>364</v>
+        <v>428</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>80</v>
+        <v>432</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>80</v>
@@ -7300,10 +7499,10 @@
         <v>80</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>80</v>
+        <v>433</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>134</v>
+        <v>434</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>80</v>
@@ -7314,10 +7513,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7325,7 +7524,7 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>91</v>
@@ -7337,23 +7536,19 @@
         <v>80</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>189</v>
+        <v>429</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="O47" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
         <v>80</v>
       </c>
@@ -7377,13 +7572,13 @@
         <v>80</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>311</v>
+        <v>80</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>427</v>
+        <v>80</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>428</v>
+        <v>80</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>80</v>
@@ -7401,16 +7596,16 @@
         <v>80</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>91</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>80</v>
+        <v>432</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>103</v>
@@ -7419,16 +7614,16 @@
         <v>80</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>429</v>
+        <v>80</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>207</v>
+        <v>433</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>208</v>
+        <v>438</v>
       </c>
       <c r="AO47" t="s" s="2">
-        <v>209</v>
+        <v>80</v>
       </c>
       <c r="AP47" t="s" s="2">
         <v>80</v>
@@ -7436,10 +7631,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7459,22 +7654,22 @@
         <v>80</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>431</v>
+        <v>189</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>268</v>
+        <v>441</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="O48" t="s" s="2">
-        <v>270</v>
+        <v>443</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>80</v>
@@ -7499,13 +7694,13 @@
         <v>80</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>80</v>
+        <v>444</v>
       </c>
       <c r="Z48" t="s" s="2">
-        <v>80</v>
+        <v>445</v>
       </c>
       <c r="AA48" t="s" s="2">
         <v>80</v>
@@ -7523,7 +7718,7 @@
         <v>80</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>78</v>
@@ -7541,27 +7736,27 @@
         <v>80</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>274</v>
+        <v>447</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>275</v>
+        <v>367</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP48" t="s" s="2">
-        <v>276</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7572,7 +7767,7 @@
         <v>78</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>80</v>
@@ -7587,16 +7782,16 @@
         <v>189</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>436</v>
+        <v>449</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>438</v>
+        <v>451</v>
       </c>
       <c r="O49" t="s" s="2">
-        <v>281</v>
+        <v>452</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>80</v>
@@ -7621,13 +7816,13 @@
         <v>80</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>282</v>
+        <v>381</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>283</v>
+        <v>453</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>284</v>
+        <v>454</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>80</v>
@@ -7645,16 +7840,16 @@
         <v>80</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>285</v>
+        <v>80</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>103</v>
@@ -7663,13 +7858,13 @@
         <v>80</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>80</v>
+        <v>446</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>134</v>
+        <v>447</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>286</v>
+        <v>367</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>80</v>
@@ -7680,21 +7875,21 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>288</v>
+        <v>80</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>80</v>
@@ -7706,19 +7901,17 @@
         <v>80</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>189</v>
+        <v>456</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>289</v>
+        <v>457</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>291</v>
-      </c>
+        <v>458</v>
+      </c>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
-        <v>292</v>
+        <v>459</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>80</v>
@@ -7743,13 +7936,13 @@
         <v>80</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>282</v>
+        <v>80</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>294</v>
+        <v>80</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>80</v>
@@ -7767,13 +7960,13 @@
         <v>80</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>80</v>
@@ -7785,27 +7978,27 @@
         <v>80</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>295</v>
+        <v>80</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>296</v>
+        <v>80</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>297</v>
+        <v>460</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP50" t="s" s="2">
-        <v>298</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>440</v>
+        <v>461</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>440</v>
+        <v>461</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7816,7 +8009,7 @@
         <v>78</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>80</v>
@@ -7828,20 +8021,16 @@
         <v>80</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>81</v>
+        <v>279</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>441</v>
+        <v>462</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="O51" t="s" s="2">
-        <v>347</v>
-      </c>
+        <v>463</v>
+      </c>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
         <v>80</v>
       </c>
@@ -7889,13 +8078,13 @@
         <v>80</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>440</v>
+        <v>461</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>80</v>
@@ -7910,20 +8099,1352 @@
         <v>80</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>349</v>
+        <v>433</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>350</v>
+        <v>464</v>
       </c>
       <c r="AO51" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP51" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" hidden="true">
+      <c r="A52" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="O52" s="2"/>
+      <c r="P52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q52" s="2"/>
+      <c r="R52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="AO52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP52" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>472</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="N53" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="O53" s="2"/>
+      <c r="P53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q53" s="2"/>
+      <c r="R53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="AO53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP53" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="B54" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="O54" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="P54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q54" s="2"/>
+      <c r="R54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="AO54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP54" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" hidden="true">
+      <c r="A55" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q55" s="2"/>
+      <c r="R55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AN55" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AO55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP55" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" hidden="true">
+      <c r="A56" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="B56" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="O56" s="2"/>
+      <c r="P56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q56" s="2"/>
+      <c r="R56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AN56" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AO56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP56" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" hidden="true">
+      <c r="A57" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="B57" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G57" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I57" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="J57" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="N57" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="O57" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="P57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q57" s="2"/>
+      <c r="R57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AN57" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AO57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP57" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" hidden="true">
+      <c r="A58" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="B58" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="G58" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J58" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K58" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>487</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="O58" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="P58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q58" s="2"/>
+      <c r="R58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X58" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="Y58" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="Z58" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="AA58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF58" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="AG58" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AH58" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ58" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL58" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="AM58" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="AN58" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="AO58" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="AP58" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" hidden="true">
+      <c r="A59" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="B59" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G59" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J59" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K59" t="s" s="2">
+        <v>494</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="N59" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="O59" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="P59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q59" s="2"/>
+      <c r="R59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF59" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="AG59" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH59" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ59" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL59" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="AM59" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AN59" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="AO59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP59" t="s" s="2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="60" hidden="true">
+      <c r="A60" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="B60" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G60" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K60" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>499</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>500</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>501</v>
+      </c>
+      <c r="O60" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="P60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q60" s="2"/>
+      <c r="R60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X60" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="Y60" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="Z60" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="AA60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF60" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="AG60" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH60" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI60" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM60" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AN60" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="AO60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP60" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" hidden="true">
+      <c r="A61" t="s" s="2">
+        <v>502</v>
+      </c>
+      <c r="B61" t="s" s="2">
+        <v>502</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G61" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K61" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="N61" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="O61" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="P61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q61" s="2"/>
+      <c r="R61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X61" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="Y61" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="Z61" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>502</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="AM61" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="AN61" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AO61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP61" t="s" s="2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="62" hidden="true">
+      <c r="A62" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="B62" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G62" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>504</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>505</v>
+      </c>
+      <c r="N62" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="O62" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="P62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q62" s="2"/>
+      <c r="R62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF62" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="AG62" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH62" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM62" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="AN62" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="AO62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP62" t="s" s="2">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP51">
+  <autoFilter ref="A1:AP62">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7933,7 +9454,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI50">
+  <conditionalFormatting sqref="A2:AI61">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>